<commit_message>
adding validation in multi excel upload page
</commit_message>
<xml_diff>
--- a/excelfile_calc/calc.xlsx
+++ b/excelfile_calc/calc.xlsx
@@ -271,7 +271,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,6 +282,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFADB9CA"/>
         <bgColor rgb="FFA8D08D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -621,7 +627,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -633,15 +639,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -677,19 +683,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -697,7 +699,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -721,7 +727,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -745,7 +751,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -773,7 +779,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="19" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2038,18 +2044,19 @@
   <dimension ref="A1:Q1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.2421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="12.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="40.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="45.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="21.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="14.94"/>

</xml_diff>